<commit_message>
v0.0.15 fix resource profile detail
</commit_message>
<xml_diff>
--- a/StructureDefinition-Vaccine-Certificate-ImmunizationRecommendation.xlsx
+++ b/StructureDefinition-Vaccine-Certificate-ImmunizationRecommendation.xlsx
@@ -2423,7 +2423,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>129</v>
       </c>
@@ -2433,13 +2433,13 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>40</v>

</xml_diff>